<commit_message>
implemented all existing changes to group_test XLSX and JS files
</commit_message>
<xml_diff>
--- a/form-files/group_test/testform.xlsx
+++ b/form-files/group_test/testform.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bennett\workspace\cse481k\AdaptiveODK\form-files\group_test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -18,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="155">
   <si>
     <t>type</t>
   </si>
@@ -438,13 +443,58 @@
   </si>
   <si>
     <t>How much does the child weigh? (kg)</t>
+  </si>
+  <si>
+    <t>section</t>
+  </si>
+  <si>
+    <t>Demographics</t>
+  </si>
+  <si>
+    <t>Danger Signs</t>
+  </si>
+  <si>
+    <t>label demographics</t>
+  </si>
+  <si>
+    <t>label general</t>
+  </si>
+  <si>
+    <t>Pneumonia</t>
+  </si>
+  <si>
+    <t>label pneumonia</t>
+  </si>
+  <si>
+    <t>label ear</t>
+  </si>
+  <si>
+    <t>parent_label</t>
+  </si>
+  <si>
+    <t>general</t>
+  </si>
+  <si>
+    <t>pneumonia</t>
+  </si>
+  <si>
+    <t>malaria_measles</t>
+  </si>
+  <si>
+    <t>ear</t>
+  </si>
+  <si>
+    <t>appearance</t>
+  </si>
+  <si>
+    <t>inline</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -457,13 +507,25 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -475,11 +537,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -491,8 +554,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -501,6 +566,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -761,7 +829,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -769,306 +837,402 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P35"/>
+  <dimension ref="A1:R39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" customWidth="1"/>
-    <col min="13" max="13" width="19.85546875" customWidth="1"/>
-    <col min="14" max="14" width="21.5703125" customWidth="1"/>
-    <col min="16" max="16" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
+    <col min="5" max="6" width="28.88671875" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" customWidth="1"/>
+    <col min="14" max="14" width="17.44140625" customWidth="1"/>
+    <col min="15" max="15" width="19.88671875" customWidth="1"/>
+    <col min="16" max="16" width="21.5546875" customWidth="1"/>
+    <col min="18" max="18" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>42</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D5" t="s">
         <v>43</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E5" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B6" s="1"/>
+      <c r="D6" t="s">
         <v>46</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E6" t="s">
         <v>139</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>26</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D7" t="s">
         <v>47</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="F7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
         <v>55</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E13" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="F13" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
-      <c r="C17" t="s">
-        <v>35</v>
+      <c r="B17" t="s">
+        <v>145</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="E17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="D18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="D19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>26</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>130</v>
+      </c>
+      <c r="D24" t="s">
         <v>61</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E24" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="F24" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>26</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D25" t="s">
         <v>63</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E25" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="F25" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>26</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D26" t="s">
         <v>65</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E26" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="F26" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>33</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D28" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="2"/>
-      <c r="P24" t="s">
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="R28" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="2"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="2"/>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1083,13 +1247,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1110,13 +1274,13 @@
       <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.140625" customWidth="1"/>
-    <col min="2" max="2" width="124.7109375" customWidth="1"/>
+    <col min="1" max="1" width="34.109375" customWidth="1"/>
+    <col min="2" max="2" width="124.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1124,7 +1288,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -1132,7 +1296,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -1140,7 +1304,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -1148,7 +1312,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>74</v>
       </c>
@@ -1156,7 +1320,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -1164,7 +1328,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>76</v>
       </c>
@@ -1172,7 +1336,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -1180,7 +1344,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -1188,7 +1352,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -1196,7 +1360,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -1204,7 +1368,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>81</v>
       </c>
@@ -1212,7 +1376,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>83</v>
       </c>
@@ -1220,7 +1384,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>82</v>
       </c>
@@ -1228,7 +1392,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>94</v>
       </c>
@@ -1236,7 +1400,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>104</v>
       </c>
@@ -1244,7 +1408,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>96</v>
       </c>
@@ -1252,7 +1416,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>101</v>
       </c>
@@ -1260,7 +1424,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>98</v>
       </c>
@@ -1268,7 +1432,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>102</v>
       </c>
@@ -1276,7 +1440,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>103</v>
       </c>
@@ -1284,7 +1448,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>105</v>
       </c>
@@ -1292,7 +1456,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>106</v>
       </c>
@@ -1300,7 +1464,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>107</v>
       </c>
@@ -1315,25 +1479,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" customWidth="1"/>
-    <col min="5" max="5" width="52.140625" customWidth="1"/>
-    <col min="6" max="6" width="54.42578125" customWidth="1"/>
-    <col min="7" max="7" width="44.85546875" customWidth="1"/>
-    <col min="8" max="8" width="28.85546875" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="3" max="4" width="27" customWidth="1"/>
+    <col min="5" max="5" width="31.88671875" customWidth="1"/>
+    <col min="6" max="6" width="52.109375" customWidth="1"/>
+    <col min="7" max="7" width="54.44140625" customWidth="1"/>
+    <col min="8" max="8" width="44.88671875" customWidth="1"/>
+    <col min="9" max="9" width="28.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -1344,22 +1508,25 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1369,9 +1536,9 @@
       <c r="C2" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1382,7 +1549,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1393,16 +1560,19 @@
         <v>38</v>
       </c>
       <c r="D4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" t="s">
         <v>108</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>125</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1413,16 +1583,19 @@
         <v>110</v>
       </c>
       <c r="D5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E5" t="s">
         <v>108</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>129</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -1433,16 +1606,19 @@
         <v>111</v>
       </c>
       <c r="D6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" t="s">
         <v>108</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>126</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1453,16 +1629,19 @@
         <v>122</v>
       </c>
       <c r="D7" t="s">
+        <v>151</v>
+      </c>
+      <c r="E7" t="s">
         <v>108</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>127</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1473,12 +1652,15 @@
         <v>130</v>
       </c>
       <c r="D8" t="s">
+        <v>152</v>
+      </c>
+      <c r="E8" t="s">
         <v>108</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>128</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1495,13 +1677,13 @@
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1510,7 +1692,7 @@
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1519,7 +1701,7 @@
       </c>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -1528,7 +1710,7 @@
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1537,32 +1719,32 @@
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>

</xml_diff>

<commit_message>
dynamic mode label in subheader
</commit_message>
<xml_diff>
--- a/form-files/group_test/testform.xlsx
+++ b/form-files/group_test/testform.xlsx
@@ -9,8 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14385" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14388" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="245">
   <si>
     <t>type</t>
   </si>
@@ -747,6 +746,18 @@
   </si>
   <si>
     <t>selected(data('anemia_pallor'))</t>
+  </si>
+  <si>
+    <t>adaptiveIMCI_commnunity</t>
+  </si>
+  <si>
+    <t>table_id</t>
+  </si>
+  <si>
+    <t>form_subtitle</t>
+  </si>
+  <si>
+    <t>Community Version</t>
   </si>
 </sst>
 </file>
@@ -1183,33 +1194,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" style="4" customWidth="1"/>
     <col min="5" max="5" width="41" style="4" customWidth="1"/>
     <col min="6" max="6" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="4"/>
-    <col min="8" max="8" width="20.7109375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="4" customWidth="1"/>
-    <col min="10" max="12" width="8.85546875" style="4"/>
-    <col min="13" max="13" width="17.28515625" style="4" customWidth="1"/>
-    <col min="14" max="15" width="8.85546875" style="4"/>
-    <col min="16" max="16" width="17.42578125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="19.85546875" style="4" customWidth="1"/>
-    <col min="18" max="18" width="21.5703125" style="4" customWidth="1"/>
-    <col min="19" max="16384" width="8.85546875" style="4"/>
+    <col min="7" max="7" width="8.88671875" style="4"/>
+    <col min="8" max="8" width="20.6640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" style="4" customWidth="1"/>
+    <col min="10" max="12" width="8.88671875" style="4"/>
+    <col min="13" max="13" width="17.33203125" style="4" customWidth="1"/>
+    <col min="14" max="15" width="8.88671875" style="4"/>
+    <col min="16" max="16" width="17.44140625" style="4" customWidth="1"/>
+    <col min="17" max="17" width="19.88671875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="21.5546875" style="4" customWidth="1"/>
+    <col min="19" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1265,7 +1272,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>141</v>
       </c>
@@ -1287,7 +1294,7 @@
       <c r="Q2" s="14"/>
       <c r="R2" s="14"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>43</v>
       </c>
@@ -1311,7 +1318,7 @@
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>23</v>
       </c>
@@ -1339,7 +1346,7 @@
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>40</v>
       </c>
@@ -1365,7 +1372,7 @@
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>23</v>
       </c>
@@ -1391,7 +1398,7 @@
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>24</v>
       </c>
@@ -1419,7 +1426,7 @@
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>48</v>
       </c>
@@ -1441,7 +1448,7 @@
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>151</v>
       </c>
@@ -1463,7 +1470,7 @@
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>43</v>
       </c>
@@ -1487,7 +1494,7 @@
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
@@ -1517,7 +1524,7 @@
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>24</v>
       </c>
@@ -1547,7 +1554,7 @@
       <c r="Q12" s="5"/>
       <c r="R12" s="5"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>24</v>
       </c>
@@ -1577,7 +1584,7 @@
       <c r="Q13" s="5"/>
       <c r="R13" s="5"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>48</v>
       </c>
@@ -1599,7 +1606,7 @@
       <c r="Q14" s="5"/>
       <c r="R14" s="5"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>43</v>
       </c>
@@ -1623,7 +1630,7 @@
       <c r="Q15" s="5"/>
       <c r="R15" s="5"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>24</v>
       </c>
@@ -1652,7 +1659,7 @@
       <c r="Q16" s="5"/>
       <c r="R16" s="5"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>24</v>
       </c>
@@ -1682,7 +1689,7 @@
       <c r="Q17" s="5"/>
       <c r="R17" s="5"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>24</v>
       </c>
@@ -1712,7 +1719,7 @@
       <c r="Q18" s="5"/>
       <c r="R18" s="5"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>24</v>
       </c>
@@ -1742,7 +1749,7 @@
       <c r="Q19" s="5"/>
       <c r="R19" s="5"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>48</v>
       </c>
@@ -1764,7 +1771,7 @@
       <c r="Q20" s="5"/>
       <c r="R20" s="5"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>143</v>
       </c>
@@ -1786,7 +1793,7 @@
       <c r="Q21" s="5"/>
       <c r="R21" s="5"/>
     </row>
-    <row r="22" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
         <v>43</v>
       </c>
@@ -1812,7 +1819,7 @@
       <c r="Q22" s="12"/>
       <c r="R22" s="12"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>154</v>
       </c>
@@ -1840,7 +1847,7 @@
       <c r="Q23" s="5"/>
       <c r="R23" s="5"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>154</v>
       </c>
@@ -1866,7 +1873,7 @@
       <c r="Q24" s="5"/>
       <c r="R24" s="5"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>24</v>
       </c>
@@ -1894,7 +1901,7 @@
       <c r="Q25" s="5"/>
       <c r="R25" s="5"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>48</v>
       </c>
@@ -1916,7 +1923,7 @@
       <c r="Q26" s="5"/>
       <c r="R26" s="5"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>160</v>
       </c>
@@ -1937,7 +1944,7 @@
       <c r="Q27" s="5"/>
       <c r="R27" s="5"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
         <v>43</v>
       </c>
@@ -1963,7 +1970,7 @@
       <c r="Q28" s="5"/>
       <c r="R28" s="5"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>154</v>
       </c>
@@ -1991,7 +1998,7 @@
       <c r="Q29" s="5"/>
       <c r="R29" s="5"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>24</v>
       </c>
@@ -2019,7 +2026,7 @@
       <c r="Q30" s="5"/>
       <c r="R30" s="5"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>24</v>
       </c>
@@ -2047,7 +2054,7 @@
       <c r="Q31" s="5"/>
       <c r="R31" s="5"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>48</v>
       </c>
@@ -2069,7 +2076,7 @@
       <c r="Q32" s="5"/>
       <c r="R32" s="5"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>204</v>
       </c>
@@ -2090,7 +2097,7 @@
       <c r="Q33" s="5"/>
       <c r="R33" s="5"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
         <v>43</v>
       </c>
@@ -2116,7 +2123,7 @@
       <c r="Q34" s="5"/>
       <c r="R34" s="5"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>154</v>
       </c>
@@ -2144,7 +2151,7 @@
       <c r="Q35" s="5"/>
       <c r="R35" s="5"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>24</v>
       </c>
@@ -2172,7 +2179,7 @@
       <c r="Q36" s="5"/>
       <c r="R36" s="5"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>24</v>
       </c>
@@ -2200,7 +2207,7 @@
       <c r="Q37" s="5"/>
       <c r="R37" s="5"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>24</v>
       </c>
@@ -2228,7 +2235,7 @@
       <c r="Q38" s="5"/>
       <c r="R38" s="5"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>24</v>
       </c>
@@ -2256,7 +2263,7 @@
       <c r="Q39" s="5"/>
       <c r="R39" s="5"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>48</v>
       </c>
@@ -2278,7 +2285,7 @@
       <c r="Q40" s="5"/>
       <c r="R40" s="5"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
         <v>43</v>
       </c>
@@ -2304,7 +2311,7 @@
       <c r="Q41" s="5"/>
       <c r="R41" s="5"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>24</v>
       </c>
@@ -2332,7 +2339,7 @@
       <c r="Q42" s="5"/>
       <c r="R42" s="5"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>24</v>
       </c>
@@ -2360,7 +2367,7 @@
       <c r="Q43" s="5"/>
       <c r="R43" s="5"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>24</v>
       </c>
@@ -2388,7 +2395,7 @@
       <c r="Q44" s="5"/>
       <c r="R44" s="5"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>48</v>
       </c>
@@ -2410,7 +2417,7 @@
       <c r="Q45" s="5"/>
       <c r="R45" s="5"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>144</v>
       </c>
@@ -2432,7 +2439,7 @@
       <c r="Q46" s="5"/>
       <c r="R46" s="5"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="12" t="s">
         <v>43</v>
       </c>
@@ -2455,7 +2462,7 @@
       <c r="Q47" s="5"/>
       <c r="R47" s="5"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>24</v>
       </c>
@@ -2483,7 +2490,7 @@
       <c r="Q48" s="5"/>
       <c r="R48" s="5"/>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>24</v>
       </c>
@@ -2511,7 +2518,7 @@
       <c r="Q49" s="5"/>
       <c r="R49" s="5"/>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>24</v>
       </c>
@@ -2539,7 +2546,7 @@
       <c r="Q50" s="5"/>
       <c r="R50" s="5"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>48</v>
       </c>
@@ -2561,7 +2568,7 @@
       <c r="Q51" s="5"/>
       <c r="R51" s="5"/>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>198</v>
       </c>
@@ -2583,7 +2590,7 @@
       <c r="Q52" s="5"/>
       <c r="R52" s="5"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" s="12" t="s">
         <v>43</v>
       </c>
@@ -2606,7 +2613,7 @@
       <c r="Q53" s="5"/>
       <c r="R53" s="5"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>24</v>
       </c>
@@ -2634,7 +2641,7 @@
       <c r="Q54" s="5"/>
       <c r="R54" s="5"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>24</v>
       </c>
@@ -2662,7 +2669,7 @@
       <c r="Q55" s="5"/>
       <c r="R55" s="5"/>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>24</v>
       </c>
@@ -2690,7 +2697,7 @@
       <c r="Q56" s="5"/>
       <c r="R56" s="5"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>24</v>
       </c>
@@ -2718,7 +2725,7 @@
       <c r="Q57" s="5"/>
       <c r="R57" s="5"/>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>48</v>
       </c>
@@ -2740,7 +2747,7 @@
       <c r="Q58" s="5"/>
       <c r="R58" s="5"/>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" s="12" t="s">
         <v>31</v>
       </c>
@@ -2768,25 +2775,25 @@
       <c r="Q59" s="5"/>
       <c r="R59" s="5"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="17"/>
       <c r="D67" s="17"/>
       <c r="E67" s="18"/>
       <c r="F67" s="18"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="17"/>
       <c r="D68" s="17"/>
       <c r="E68" s="18"/>
       <c r="F68" s="18"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="17"/>
       <c r="D69" s="17"/>
       <c r="E69" s="18"/>
       <c r="F69" s="18"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="17"/>
       <c r="D70" s="17"/>
       <c r="E70" s="18"/>
@@ -2802,20 +2809,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="5" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="5"/>
+    <col min="1" max="1" width="17.33203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="5" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
@@ -2832,23 +2835,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29" style="2" customWidth="1"/>
-    <col min="2" max="2" width="97.42578125" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="97.44140625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
@@ -2856,8 +2855,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>67</v>
       </c>
@@ -2865,7 +2864,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>66</v>
       </c>
@@ -2873,7 +2872,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>206</v>
       </c>
@@ -2881,7 +2880,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>68</v>
       </c>
@@ -2889,7 +2888,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>72</v>
       </c>
@@ -2897,7 +2896,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>73</v>
       </c>
@@ -2905,7 +2904,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>74</v>
       </c>
@@ -2913,7 +2912,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>75</v>
       </c>
@@ -2921,7 +2920,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>76</v>
       </c>
@@ -2929,7 +2928,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>77</v>
       </c>
@@ -2937,7 +2936,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>78</v>
       </c>
@@ -2945,7 +2944,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>208</v>
       </c>
@@ -2953,7 +2952,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>211</v>
       </c>
@@ -2961,7 +2960,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>214</v>
       </c>
@@ -2969,7 +2968,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>216</v>
       </c>
@@ -2977,7 +2976,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>218</v>
       </c>
@@ -2985,7 +2984,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>221</v>
       </c>
@@ -2993,7 +2992,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>224</v>
       </c>
@@ -3001,7 +3000,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>226</v>
       </c>
@@ -3009,7 +3008,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>77</v>
       </c>
@@ -3017,7 +3016,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>229</v>
       </c>
@@ -3025,7 +3024,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>231</v>
       </c>
@@ -3033,7 +3032,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>79</v>
       </c>
@@ -3041,7 +3040,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>81</v>
       </c>
@@ -3049,7 +3048,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>80</v>
       </c>
@@ -3057,7 +3056,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>234</v>
       </c>
@@ -3065,7 +3064,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>235</v>
       </c>
@@ -3073,7 +3072,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>237</v>
       </c>
@@ -3081,7 +3080,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>239</v>
       </c>
@@ -3089,7 +3088,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>92</v>
       </c>
@@ -3097,7 +3096,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>102</v>
       </c>
@@ -3105,7 +3104,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>94</v>
       </c>
@@ -3113,7 +3112,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>99</v>
       </c>
@@ -3121,7 +3120,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>96</v>
       </c>
@@ -3129,7 +3128,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>202</v>
       </c>
@@ -3137,7 +3136,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>100</v>
       </c>
@@ -3145,7 +3144,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>101</v>
       </c>
@@ -3153,7 +3152,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>103</v>
       </c>
@@ -3161,7 +3160,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>104</v>
       </c>
@@ -3169,7 +3168,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>105</v>
       </c>
@@ -3177,7 +3176,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>200</v>
       </c>
@@ -3194,25 +3193,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
     <col min="3" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" customWidth="1"/>
-    <col min="6" max="6" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="54.42578125" customWidth="1"/>
-    <col min="8" max="8" width="44.85546875" customWidth="1"/>
-    <col min="9" max="9" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="31.88671875" customWidth="1"/>
+    <col min="6" max="6" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.44140625" customWidth="1"/>
+    <col min="8" max="8" width="44.88671875" customWidth="1"/>
+    <col min="9" max="9" width="28.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -3241,7 +3236,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>25</v>
       </c>
@@ -3258,7 +3253,7 @@
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>25</v>
       </c>
@@ -3275,7 +3270,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>35</v>
       </c>
@@ -3300,7 +3295,7 @@
       </c>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>35</v>
       </c>
@@ -3325,7 +3320,7 @@
       </c>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
@@ -3350,7 +3345,7 @@
       </c>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>35</v>
       </c>
@@ -3375,7 +3370,7 @@
       </c>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>35</v>
       </c>
@@ -3400,7 +3395,7 @@
       </c>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>35</v>
       </c>
@@ -3432,20 +3427,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25" style="6" customWidth="1"/>
     <col min="2" max="2" width="24" style="6" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="6"/>
+    <col min="3" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="8" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>15</v>
       </c>
@@ -3454,59 +3445,67 @@
       </c>
       <c r="C1" s="9"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C2" s="7"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>0.5</v>
       </c>
-      <c r="C3" s="7"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="C4" s="7"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
       <c r="C5" s="7"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>244</v>
+      </c>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>

</xml_diff>